<commit_message>
weekly update, script improvements
</commit_message>
<xml_diff>
--- a/data/BI_SPE_raw.xlsx
+++ b/data/BI_SPE_raw.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RetnoAndrini\Departemen Statistik\Survei\SPE\2020\10. Oktober\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_hasyim\Desktop\BIWEB\arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel 1" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="106">
   <si>
     <t>DESKRIPSI</t>
   </si>
@@ -558,19 +558,16 @@
   <si>
     <t>Makassar</t>
   </si>
-  <si>
-    <t>Nov*</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1432,7 +1429,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1441,7 +1438,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1462,7 +1459,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1478,24 +1475,24 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1516,7 +1513,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1530,7 +1527,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1542,7 +1539,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1560,37 +1557,37 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1617,13 +1614,13 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1635,7 +1632,7 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1650,16 +1647,16 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1668,9 +1665,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
@@ -1720,35 +1717,35 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5247,17 +5244,16 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC5" sqref="DC5:DD5"/>
+      <selection pane="topRight" activeCell="DD6" sqref="DD6:DE14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="62" width="9.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="9.36328125" customWidth="1" collapsed="1"/>
-    <col min="64" max="108" width="9.36328125" customWidth="1"/>
-    <col min="109" max="109" width="9.36328125" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="43.36328125" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="62" width="9.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="64" max="109" width="9.33203125" customWidth="1"/>
+    <col min="110" max="110" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:110" s="16" customFormat="1" ht="16.5" customHeight="1">
@@ -5942,7 +5938,7 @@
         <v>9</v>
       </c>
       <c r="DD5" s="50" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="DE5" s="51" t="s">
         <v>86</v>
@@ -6349,9 +6345,11 @@
         <v>118.70683440497544</v>
       </c>
       <c r="DD6" s="54">
-        <v>121.51089017057114</v>
-      </c>
-      <c r="DE6" s="54"/>
+        <v>121.07870215026861</v>
+      </c>
+      <c r="DE6" s="54">
+        <v>125.47633379950062</v>
+      </c>
       <c r="DF6" s="66" t="s">
         <v>56</v>
       </c>
@@ -6756,9 +6754,11 @@
         <v>222.74394900394017</v>
       </c>
       <c r="DD7" s="58">
-        <v>221.73405308703073</v>
-      </c>
-      <c r="DE7" s="58"/>
+        <v>221.55915020118832</v>
+      </c>
+      <c r="DE7" s="58">
+        <v>226.89880585750427</v>
+      </c>
       <c r="DF7" s="67" t="s">
         <v>24</v>
       </c>
@@ -7163,9 +7163,11 @@
         <v>71.029015258345865</v>
       </c>
       <c r="DD8" s="54">
-        <v>73.348072308849268</v>
-      </c>
-      <c r="DE8" s="54"/>
+        <v>73.269386221438481</v>
+      </c>
+      <c r="DE8" s="54">
+        <v>75.5457301793151</v>
+      </c>
       <c r="DF8" s="66" t="s">
         <v>25</v>
       </c>
@@ -7570,9 +7572,11 @@
         <v>212.706196602604</v>
       </c>
       <c r="DD9" s="58">
-        <v>206.48834183426487</v>
-      </c>
-      <c r="DE9" s="58"/>
+        <v>199.56073267181466</v>
+      </c>
+      <c r="DE9" s="58">
+        <v>208.60787734514153</v>
+      </c>
       <c r="DF9" s="67" t="s">
         <v>26</v>
       </c>
@@ -7977,9 +7981,11 @@
         <v>132.48074363720579</v>
       </c>
       <c r="DD10" s="54">
-        <v>131.93488150342881</v>
-      </c>
-      <c r="DE10" s="54"/>
+        <v>127.49047950773279</v>
+      </c>
+      <c r="DE10" s="54">
+        <v>131.25233965858175</v>
+      </c>
       <c r="DF10" s="66" t="s">
         <v>27</v>
       </c>
@@ -8384,9 +8390,11 @@
         <v>65.04038876002133</v>
       </c>
       <c r="DD11" s="58">
-        <v>64.291758693644482</v>
-      </c>
-      <c r="DE11" s="58"/>
+        <v>64.974398873641434</v>
+      </c>
+      <c r="DE11" s="58">
+        <v>66.349140861012771</v>
+      </c>
       <c r="DF11" s="67" t="s">
         <v>28</v>
       </c>
@@ -8791,9 +8799,11 @@
         <v>77.731931582534358</v>
       </c>
       <c r="DD12" s="54">
-        <v>79.38430263237197</v>
-      </c>
-      <c r="DE12" s="54"/>
+        <v>78.877852328227178</v>
+      </c>
+      <c r="DE12" s="54">
+        <v>83.394912687695211</v>
+      </c>
       <c r="DF12" s="66" t="s">
         <v>29</v>
       </c>
@@ -9198,9 +9208,11 @@
         <v>66.348474315797517</v>
       </c>
       <c r="DD13" s="58">
-        <v>69.517679400867394</v>
-      </c>
-      <c r="DE13" s="58"/>
+        <v>70.598412242379766</v>
+      </c>
+      <c r="DE13" s="58">
+        <v>73.780161581001735</v>
+      </c>
       <c r="DF13" s="67" t="s">
         <v>30</v>
       </c>
@@ -9605,9 +9617,11 @@
         <v>183.47160216961299</v>
       </c>
       <c r="DD14" s="115">
-        <v>182.66497428989769</v>
-      </c>
-      <c r="DE14" s="115"/>
+        <v>181.33573874918136</v>
+      </c>
+      <c r="DE14" s="115">
+        <v>186.53135249313951</v>
+      </c>
       <c r="DF14" s="68" t="s">
         <v>31</v>
       </c>
@@ -9844,7 +9858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:110" s="30" customFormat="1" ht="13.5">
+    <row r="17" spans="1:110" s="30" customFormat="1" ht="13.2">
       <c r="A17" s="22" t="s">
         <v>81</v>
       </c>
@@ -9878,25 +9892,24 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC5" sqref="DC5:DD5"/>
+      <selection pane="topRight" activeCell="DD6" sqref="DD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="38" width="9.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="61" width="9.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="9.36328125" customWidth="1" collapsed="1"/>
-    <col min="63" max="73" width="9.36328125" customWidth="1"/>
-    <col min="74" max="75" width="8.453125" customWidth="1"/>
-    <col min="76" max="76" width="8.36328125" customWidth="1"/>
-    <col min="77" max="77" width="5.90625" customWidth="1"/>
-    <col min="79" max="79" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="38" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="61" width="9.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="63" max="73" width="9.33203125" customWidth="1"/>
+    <col min="74" max="75" width="8.44140625" customWidth="1"/>
+    <col min="76" max="76" width="8.33203125" customWidth="1"/>
+    <col min="77" max="77" width="5.88671875" customWidth="1"/>
+    <col min="79" max="79" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="80" max="100" width="7" customWidth="1"/>
-    <col min="101" max="101" width="7.08984375" customWidth="1"/>
-    <col min="102" max="108" width="7" customWidth="1"/>
-    <col min="109" max="109" width="7" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="45.36328125" customWidth="1"/>
+    <col min="101" max="101" width="7.109375" customWidth="1"/>
+    <col min="102" max="109" width="7" customWidth="1"/>
+    <col min="110" max="110" width="45.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:112" s="16" customFormat="1" ht="16.5" customHeight="1">
@@ -10515,7 +10528,7 @@
         <v>9</v>
       </c>
       <c r="DD5" s="50" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="DE5" s="51" t="s">
         <v>86</v>
@@ -10940,11 +10953,11 @@
       </c>
       <c r="DD6" s="54">
         <f>IFERROR('Tabel 1'!DD6/'Tabel 1'!CR6*100-100,"")</f>
-        <v>-21.339335412028433</v>
+        <v>-21.619114424890867</v>
       </c>
       <c r="DE6" s="54">
         <f>IFERROR('Tabel 1'!DE6/'Tabel 1'!CS6*100-100,"")</f>
-        <v>-100</v>
+        <v>-19.990262001134724</v>
       </c>
       <c r="DF6" s="66" t="s">
         <v>56</v>
@@ -11368,11 +11381,11 @@
       </c>
       <c r="DD7" s="58">
         <f>IFERROR('Tabel 1'!DD7/'Tabel 1'!CR7*100-100,"")</f>
-        <v>-6.5066320569849836</v>
+        <v>-6.5803792312809577</v>
       </c>
       <c r="DE7" s="58">
         <f>IFERROR('Tabel 1'!DE7/'Tabel 1'!CS7*100-100,"")</f>
-        <v>-100</v>
+        <v>-12.321549583570118</v>
       </c>
       <c r="DF7" s="67" t="s">
         <v>24</v>
@@ -11796,11 +11809,11 @@
       </c>
       <c r="DD8" s="54">
         <f>IFERROR('Tabel 1'!DD8/'Tabel 1'!CR8*100-100,"")</f>
-        <v>-14.176656191744271</v>
+        <v>-14.268725457100658</v>
       </c>
       <c r="DE8" s="54">
         <f>IFERROR('Tabel 1'!DE8/'Tabel 1'!CS8*100-100,"")</f>
-        <v>-100</v>
+        <v>-12.175824269573695</v>
       </c>
       <c r="DF8" s="66" t="s">
         <v>25</v>
@@ -12224,11 +12237,11 @@
       </c>
       <c r="DD9" s="58">
         <f>IFERROR('Tabel 1'!DD9/'Tabel 1'!CR9*100-100,"")</f>
-        <v>-34.04230551916126</v>
+        <v>-36.255162305944388</v>
       </c>
       <c r="DE9" s="58">
         <f>IFERROR('Tabel 1'!DE9/'Tabel 1'!CS9*100-100,"")</f>
-        <v>-100</v>
+        <v>-38.434248129534751</v>
       </c>
       <c r="DF9" s="67" t="s">
         <v>26</v>
@@ -12652,11 +12665,11 @@
       </c>
       <c r="DD10" s="54">
         <f>IFERROR('Tabel 1'!DD10/'Tabel 1'!CR10*100-100,"")</f>
-        <v>-23.761909835487899</v>
+        <v>-26.330091321794882</v>
       </c>
       <c r="DE10" s="54">
         <f>IFERROR('Tabel 1'!DE10/'Tabel 1'!CS10*100-100,"")</f>
-        <v>-100</v>
+        <v>-27.83789797849137</v>
       </c>
       <c r="DF10" s="66" t="s">
         <v>27</v>
@@ -13080,11 +13093,11 @@
       </c>
       <c r="DD11" s="58">
         <f>IFERROR('Tabel 1'!DD11/'Tabel 1'!CR11*100-100,"")</f>
-        <v>-40.968713580553654</v>
+        <v>-40.341928300361808</v>
       </c>
       <c r="DE11" s="58">
         <f>IFERROR('Tabel 1'!DE11/'Tabel 1'!CS11*100-100,"")</f>
-        <v>-100</v>
+        <v>-38.573065030764923</v>
       </c>
       <c r="DF11" s="67" t="s">
         <v>28</v>
@@ -13508,11 +13521,11 @@
       </c>
       <c r="DD12" s="54">
         <f>IFERROR('Tabel 1'!DD12/'Tabel 1'!CR12*100-100,"")</f>
-        <v>-50.980532459498072</v>
+        <v>-51.293263357442356</v>
       </c>
       <c r="DE12" s="54">
         <f>IFERROR('Tabel 1'!DE12/'Tabel 1'!CS12*100-100,"")</f>
-        <v>-100</v>
+        <v>-55.923079774234211</v>
       </c>
       <c r="DF12" s="66" t="s">
         <v>29</v>
@@ -13936,11 +13949,11 @@
       </c>
       <c r="DD13" s="58">
         <f>IFERROR('Tabel 1'!DD13/'Tabel 1'!CR13*100-100,"")</f>
-        <v>-57.300322121238672</v>
+        <v>-56.636506173938784</v>
       </c>
       <c r="DE13" s="58">
         <f>IFERROR('Tabel 1'!DE13/'Tabel 1'!CS13*100-100,"")</f>
-        <v>-100</v>
+        <v>-60.891645795147845</v>
       </c>
       <c r="DF13" s="67" t="s">
         <v>30</v>
@@ -14364,11 +14377,11 @@
       </c>
       <c r="DD14" s="62">
         <f>IFERROR('Tabel 1'!DD14/'Tabel 1'!CR14*100-100,"")</f>
-        <v>-15.659859886113878</v>
+        <v>-16.273595016147354</v>
       </c>
       <c r="DE14" s="62">
         <f>IFERROR('Tabel 1'!DE14/'Tabel 1'!CS14*100-100,"")</f>
-        <v>-100</v>
+        <v>-20.658013732269211</v>
       </c>
       <c r="DF14" s="68" t="s">
         <v>31</v>
@@ -14608,7 +14621,7 @@
       <c r="DG16" s="29"/>
       <c r="DH16" s="29"/>
     </row>
-    <row r="17" spans="1:110" s="30" customFormat="1" ht="13.5">
+    <row r="17" spans="1:110" s="30" customFormat="1" ht="13.2">
       <c r="A17" s="22" t="s">
         <v>81</v>
       </c>
@@ -14640,22 +14653,21 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC5" sqref="DC5:DD5"/>
+      <selection pane="topRight" activeCell="DD6" sqref="DD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="38" width="9.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="61" width="9.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="9.36328125" customWidth="1" collapsed="1"/>
-    <col min="63" max="73" width="9.36328125" customWidth="1"/>
-    <col min="74" max="75" width="8.54296875" customWidth="1"/>
-    <col min="76" max="76" width="8.6328125" customWidth="1"/>
-    <col min="77" max="77" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="80" max="108" width="9.08984375" customWidth="1"/>
-    <col min="109" max="109" width="9.08984375" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="43.08984375" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="38" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="61" width="9.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="63" max="73" width="9.33203125" customWidth="1"/>
+    <col min="74" max="75" width="8.5546875" customWidth="1"/>
+    <col min="76" max="76" width="8.6640625" customWidth="1"/>
+    <col min="77" max="77" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="109" width="9.109375" customWidth="1"/>
+    <col min="110" max="110" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:110" s="16" customFormat="1" ht="16.5" customHeight="1">
@@ -15273,7 +15285,7 @@
         <v>9</v>
       </c>
       <c r="DD5" s="50" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="DE5" s="51" t="s">
         <v>86</v>
@@ -15709,11 +15721,11 @@
       </c>
       <c r="DD6" s="54">
         <f>IFERROR('Tabel 1'!DD6/'Tabel 1'!DC6*100-100,"")</f>
-        <v>2.3621687661466098</v>
+        <v>1.9980886165335647</v>
       </c>
       <c r="DE6" s="54">
         <f>IFERROR('Tabel 1'!DE6/'Tabel 1'!DD6*100-100,"")</f>
-        <v>-100</v>
+        <v>3.6320439277373566</v>
       </c>
       <c r="DF6" s="66" t="s">
         <v>56</v>
@@ -16148,11 +16160,11 @@
       </c>
       <c r="DD7" s="58">
         <f>IFERROR('Tabel 1'!DD7/'Tabel 1'!DC7*100-100,"")</f>
-        <v>-0.45338870996292258</v>
+        <v>-0.53191065707957819</v>
       </c>
       <c r="DE7" s="58">
         <f>IFERROR('Tabel 1'!DE7/'Tabel 1'!DD7*100-100,"")</f>
-        <v>-100</v>
+        <v>2.4100361693332246</v>
       </c>
       <c r="DF7" s="67" t="s">
         <v>24</v>
@@ -16587,11 +16599,11 @@
       </c>
       <c r="DD8" s="54">
         <f>IFERROR('Tabel 1'!DD8/'Tabel 1'!DC8*100-100,"")</f>
-        <v>3.2649432658872684</v>
+        <v>3.1541630627201585</v>
       </c>
       <c r="DE8" s="54">
         <f>IFERROR('Tabel 1'!DE8/'Tabel 1'!DD8*100-100,"")</f>
-        <v>-100</v>
+        <v>3.1068145582616751</v>
       </c>
       <c r="DF8" s="66" t="s">
         <v>25</v>
@@ -17026,11 +17038,11 @@
       </c>
       <c r="DD9" s="58">
         <f>IFERROR('Tabel 1'!DD9/'Tabel 1'!DC9*100-100,"")</f>
-        <v>-2.9232128013439365</v>
+        <v>-6.1801038901319885</v>
       </c>
       <c r="DE9" s="58">
         <f>IFERROR('Tabel 1'!DE9/'Tabel 1'!DD9*100-100,"")</f>
-        <v>-100</v>
+        <v>4.5335294936029555</v>
       </c>
       <c r="DF9" s="67" t="s">
         <v>26</v>
@@ -17465,11 +17477,11 @@
       </c>
       <c r="DD10" s="54">
         <f>IFERROR('Tabel 1'!DD10/'Tabel 1'!DC10*100-100,"")</f>
-        <v>-0.4120313026561746</v>
+        <v>-3.766784509557624</v>
       </c>
       <c r="DE10" s="54">
         <f>IFERROR('Tabel 1'!DE10/'Tabel 1'!DD10*100-100,"")</f>
-        <v>-100</v>
+        <v>2.9506988799275575</v>
       </c>
       <c r="DF10" s="66" t="s">
         <v>27</v>
@@ -17904,11 +17916,11 @@
       </c>
       <c r="DD11" s="58">
         <f>IFERROR('Tabel 1'!DD11/'Tabel 1'!DC11*100-100,"")</f>
-        <v>-1.1510233574080502</v>
+        <v>-0.10145985846328642</v>
       </c>
       <c r="DE11" s="58">
         <f>IFERROR('Tabel 1'!DE11/'Tabel 1'!DD11*100-100,"")</f>
-        <v>-100</v>
+        <v>2.1158210175131558</v>
       </c>
       <c r="DF11" s="67" t="s">
         <v>28</v>
@@ -18343,11 +18355,11 @@
       </c>
       <c r="DD12" s="54">
         <f>IFERROR('Tabel 1'!DD12/'Tabel 1'!DC12*100-100,"")</f>
-        <v>2.1257300779707862</v>
+        <v>1.4741956392478244</v>
       </c>
       <c r="DE12" s="54">
         <f>IFERROR('Tabel 1'!DE12/'Tabel 1'!DD12*100-100,"")</f>
-        <v>-100</v>
+        <v>5.7266523189191361</v>
       </c>
       <c r="DF12" s="66" t="s">
         <v>29</v>
@@ -18782,11 +18794,11 @@
       </c>
       <c r="DD13" s="58">
         <f>IFERROR('Tabel 1'!DD13/'Tabel 1'!DC13*100-100,"")</f>
-        <v>4.7766058191262744</v>
+        <v>6.4054795086227614</v>
       </c>
       <c r="DE13" s="58">
         <f>IFERROR('Tabel 1'!DE13/'Tabel 1'!DD13*100-100,"")</f>
-        <v>-100</v>
+        <v>4.5068284647795167</v>
       </c>
       <c r="DF13" s="67" t="s">
         <v>30</v>
@@ -19221,11 +19233,11 @@
       </c>
       <c r="DD14" s="62">
         <f>IFERROR('Tabel 1'!DD14/'Tabel 1'!DC14*100-100,"")</f>
-        <v>-0.43964726430503731</v>
+        <v>-1.16413842533359</v>
       </c>
       <c r="DE14" s="62">
         <f>IFERROR('Tabel 1'!DE14/'Tabel 1'!DD14*100-100,"")</f>
-        <v>-100</v>
+        <v>2.8651901604154233</v>
       </c>
       <c r="DF14" s="68" t="s">
         <v>31</v>
@@ -19494,21 +19506,20 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ1" sqref="AJ1:AL1048576"/>
+      <selection pane="topRight" activeCell="AK6" sqref="AK6:AK14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="21" width="8.90625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.08984375" collapsed="1"/>
-    <col min="24" max="25" width="8.08984375" customWidth="1"/>
-    <col min="26" max="36" width="7.54296875" style="48" customWidth="1"/>
-    <col min="37" max="37" width="7.54296875" style="48" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="43.36328125" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="21" width="8.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.109375" collapsed="1"/>
+    <col min="24" max="25" width="8.109375" customWidth="1"/>
+    <col min="26" max="37" width="7.5546875" style="48" customWidth="1"/>
+    <col min="38" max="38" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" s="16" customFormat="1" ht="16.25" customHeight="1">
+    <row r="2" spans="1:38" s="16" customFormat="1" ht="16.2" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>94</v>
       </c>
@@ -19903,7 +19914,9 @@
         <f>AVERAGE('Tabel 2'!CZ6:DB6)</f>
         <v>-27.419652442326694</v>
       </c>
-      <c r="AK6" s="54"/>
+      <c r="AK6" s="54">
+        <v>-21.486589390819045</v>
+      </c>
       <c r="AL6" s="66" t="s">
         <v>56</v>
       </c>
@@ -20046,7 +20059,9 @@
         <f>AVERAGE('Tabel 2'!CZ7:DB7)</f>
         <v>1.2833176182434585</v>
       </c>
-      <c r="AK7" s="58"/>
+      <c r="AK7" s="58">
+        <v>-8.1509996211670828</v>
+      </c>
       <c r="AL7" s="67" t="s">
         <v>24</v>
       </c>
@@ -20189,7 +20204,9 @@
         <f>AVERAGE('Tabel 2'!CZ8:DB8)</f>
         <v>-22.763319688511718</v>
       </c>
-      <c r="AK8" s="54"/>
+      <c r="AK8" s="54">
+        <v>-14.56924510091774</v>
+      </c>
       <c r="AL8" s="66" t="s">
         <v>25</v>
       </c>
@@ -20332,7 +20349,9 @@
         <f>AVERAGE('Tabel 2'!CZ9:DB9)</f>
         <v>-19.573840590952482</v>
       </c>
-      <c r="AK9" s="58"/>
+      <c r="AK9" s="58">
+        <v>-35.200904649497467</v>
+      </c>
       <c r="AL9" s="67" t="s">
         <v>26</v>
       </c>
@@ -20475,7 +20494,9 @@
         <f>AVERAGE('Tabel 2'!CZ10:DB10)</f>
         <v>-24.020977310172452</v>
       </c>
-      <c r="AK10" s="54"/>
+      <c r="AK10" s="54">
+        <v>-25.831552553040979</v>
+      </c>
       <c r="AL10" s="66" t="s">
         <v>27</v>
       </c>
@@ -20618,7 +20639,9 @@
         <f>AVERAGE('Tabel 2'!CZ11:DB11)</f>
         <v>-38.814308944170598</v>
       </c>
-      <c r="AK11" s="58"/>
+      <c r="AK11" s="58">
+        <v>-39.825321659563038</v>
+      </c>
       <c r="AL11" s="67" t="s">
         <v>28</v>
       </c>
@@ -20761,7 +20784,9 @@
         <f>AVERAGE('Tabel 2'!CZ12:DB12)</f>
         <v>-56.261275711607801</v>
       </c>
-      <c r="AK12" s="54"/>
+      <c r="AK12" s="54">
+        <v>-53.576708830134777</v>
+      </c>
       <c r="AL12" s="66" t="s">
         <v>29</v>
       </c>
@@ -20904,7 +20929,9 @@
         <f>AVERAGE('Tabel 2'!CZ13:DB13)</f>
         <v>-63.685757994892349</v>
       </c>
-      <c r="AK13" s="58"/>
+      <c r="AK13" s="58">
+        <v>-58.531668065255296</v>
+      </c>
       <c r="AL13" s="67" t="s">
         <v>30</v>
       </c>
@@ -21047,7 +21074,9 @@
         <f>AVERAGE('Tabel 2'!CZ14:DB14)</f>
         <v>-10.06733208233031</v>
       </c>
-      <c r="AK14" s="123"/>
+      <c r="AK14" s="123">
+        <v>-17.292126116453691</v>
+      </c>
       <c r="AL14" s="68" t="s">
         <v>31</v>
       </c>
@@ -21296,21 +21325,20 @@
       <pane xSplit="1" ySplit="5" topLeftCell="CU6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="DA18" sqref="DA18"/>
+      <selection pane="bottomRight" activeCell="DD6" sqref="DD6:DE15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="35.90625" customWidth="1"/>
-    <col min="2" max="60" width="9.36328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="5.6328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="9.36328125" customWidth="1" collapsed="1"/>
-    <col min="63" max="91" width="9.36328125" customWidth="1"/>
-    <col min="92" max="92" width="10.1796875" customWidth="1"/>
-    <col min="93" max="108" width="9.36328125" customWidth="1"/>
-    <col min="109" max="109" width="9.36328125" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="42.08984375" style="34" customWidth="1"/>
-    <col min="113" max="113" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="2" max="60" width="9.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="5.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="9.33203125" customWidth="1" collapsed="1"/>
+    <col min="63" max="91" width="9.33203125" customWidth="1"/>
+    <col min="92" max="92" width="10.21875" customWidth="1"/>
+    <col min="93" max="109" width="9.33203125" customWidth="1"/>
+    <col min="110" max="110" width="42.109375" style="34" customWidth="1"/>
+    <col min="113" max="113" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:148" s="16" customFormat="1" ht="15" customHeight="1">
@@ -22033,7 +22061,7 @@
         <v>9</v>
       </c>
       <c r="DD5" s="50" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="DE5" s="51" t="s">
         <v>86</v>
@@ -22363,9 +22391,11 @@
         <v>56.448893951502534</v>
       </c>
       <c r="DD6" s="54">
-        <v>58.790047849981377</v>
-      </c>
-      <c r="DE6" s="54"/>
+        <v>58.180063316059247</v>
+      </c>
+      <c r="DE6" s="54">
+        <v>64.380644556199314</v>
+      </c>
       <c r="DF6" s="64" t="s">
         <v>39</v>
       </c>
@@ -22693,9 +22723,11 @@
         <v>179.99227270494185</v>
       </c>
       <c r="DD7" s="58">
-        <v>171.50103084730679</v>
-      </c>
-      <c r="DE7" s="58"/>
+        <v>171.20183363550152</v>
+      </c>
+      <c r="DE7" s="58">
+        <v>172.84653113170484</v>
+      </c>
       <c r="DF7" s="65" t="s">
         <v>40</v>
       </c>
@@ -23023,9 +23055,11 @@
         <v>283.30880376148826</v>
       </c>
       <c r="DD8" s="54">
-        <v>291.72653394607391</v>
-      </c>
-      <c r="DE8" s="54"/>
+        <v>293.90113965441299</v>
+      </c>
+      <c r="DE8" s="54">
+        <v>302.5493684757954</v>
+      </c>
       <c r="DF8" s="64" t="s">
         <v>41</v>
       </c>
@@ -23353,9 +23387,11 @@
         <v>161.41273948354348</v>
       </c>
       <c r="DD9" s="58">
-        <v>165.95894250063725</v>
-      </c>
-      <c r="DE9" s="58"/>
+        <v>164.32585634268631</v>
+      </c>
+      <c r="DE9" s="58">
+        <v>169.69556363304415</v>
+      </c>
       <c r="DF9" s="65" t="s">
         <v>42</v>
       </c>
@@ -23683,9 +23719,11 @@
         <v>120.51543084843507</v>
       </c>
       <c r="DD10" s="54">
-        <v>118.31580264877235</v>
-      </c>
-      <c r="DE10" s="54"/>
+        <v>111.07592968194322</v>
+      </c>
+      <c r="DE10" s="54">
+        <v>116.20926105684346</v>
+      </c>
       <c r="DF10" s="64" t="s">
         <v>43</v>
       </c>
@@ -24013,9 +24051,11 @@
         <v>93.04565293773426</v>
       </c>
       <c r="DD11" s="58">
-        <v>97.323867616954786</v>
-      </c>
-      <c r="DE11" s="58"/>
+        <v>92.147049412221008</v>
+      </c>
+      <c r="DE11" s="58">
+        <v>98.330061850608516</v>
+      </c>
       <c r="DF11" s="65" t="s">
         <v>44</v>
       </c>
@@ -24343,9 +24383,11 @@
         <v>182.3056352185942</v>
       </c>
       <c r="DD12" s="54">
-        <v>184.10655345622501</v>
-      </c>
-      <c r="DE12" s="54"/>
+        <v>180.86604495460239</v>
+      </c>
+      <c r="DE12" s="54">
+        <v>184.74035454190755</v>
+      </c>
       <c r="DF12" s="64" t="s">
         <v>45</v>
       </c>
@@ -24673,9 +24715,11 @@
         <v>196.443191590705</v>
       </c>
       <c r="DD13" s="58">
-        <v>199.26896542728653</v>
-      </c>
-      <c r="DE13" s="58"/>
+        <v>201.41169750047854</v>
+      </c>
+      <c r="DE13" s="58">
+        <v>210.72019271230906</v>
+      </c>
       <c r="DF13" s="65" t="s">
         <v>46</v>
       </c>
@@ -25003,9 +25047,11 @@
         <v>92.519594354496121</v>
       </c>
       <c r="DD14" s="54">
-        <v>92.167936814518796</v>
-      </c>
-      <c r="DE14" s="54"/>
+        <v>91.802951639540055</v>
+      </c>
+      <c r="DE14" s="54">
+        <v>92.5000264090841</v>
+      </c>
       <c r="DF14" s="64" t="s">
         <v>47</v>
       </c>
@@ -25333,9 +25379,11 @@
         <v>183.47160216961299</v>
       </c>
       <c r="DD15" s="115">
-        <v>182.66497428989769</v>
-      </c>
-      <c r="DE15" s="115"/>
+        <v>181.33573874918136</v>
+      </c>
+      <c r="DE15" s="115">
+        <v>186.53135249313951</v>
+      </c>
       <c r="DF15" s="79" t="s">
         <v>31</v>
       </c>
@@ -25782,20 +25830,19 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC5" sqref="DC5:DD5"/>
+      <selection pane="topRight" activeCell="DD6" sqref="DD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="61" width="9.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="8.90625" collapsed="1"/>
-    <col min="74" max="75" width="8.6328125" customWidth="1"/>
-    <col min="76" max="76" width="7.6328125" customWidth="1"/>
-    <col min="77" max="77" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="80" max="108" width="9.08984375" customWidth="1"/>
-    <col min="109" max="109" width="9.08984375" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="28.90625" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="61" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="8.88671875" collapsed="1"/>
+    <col min="74" max="75" width="8.6640625" customWidth="1"/>
+    <col min="76" max="76" width="7.6640625" customWidth="1"/>
+    <col min="77" max="77" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="80" max="109" width="9.109375" customWidth="1"/>
+    <col min="110" max="110" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:110" s="16" customFormat="1" ht="15" customHeight="1">
@@ -25881,7 +25928,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:110" ht="17" customHeight="1" thickBot="1">
+    <row r="3" spans="1:110" ht="16.95" customHeight="1" thickBot="1">
       <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -26414,7 +26461,7 @@
         <v>9</v>
       </c>
       <c r="DD5" s="50" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="DE5" s="50" t="s">
         <v>86</v>
@@ -26839,11 +26886,11 @@
       </c>
       <c r="DD6" s="54">
         <f>IFERROR('Tabel 5'!DD6/'Tabel 5'!CR6*100-100,"")</f>
-        <v>-45.219699364358725</v>
+        <v>-45.788080193655091</v>
       </c>
       <c r="DE6" s="54">
         <f>IFERROR('Tabel 5'!DE6/'Tabel 5'!CS6*100-100,"")</f>
-        <v>-100</v>
+        <v>-48.852546370883928</v>
       </c>
       <c r="DF6" s="66" t="s">
         <v>39</v>
@@ -27267,11 +27314,11 @@
       </c>
       <c r="DD7" s="58">
         <f>IFERROR('Tabel 5'!DD7/'Tabel 5'!CR7*100-100,"")</f>
-        <v>-29.204757822316637</v>
+        <v>-29.328265762554622</v>
       </c>
       <c r="DE7" s="58">
         <f>IFERROR('Tabel 5'!DE7/'Tabel 5'!CS7*100-100,"")</f>
-        <v>-100</v>
+        <v>-33.911539990860206</v>
       </c>
       <c r="DF7" s="67" t="s">
         <v>40</v>
@@ -27695,11 +27742,11 @@
       </c>
       <c r="DD8" s="54">
         <f>IFERROR('Tabel 5'!DD8/'Tabel 5'!CR8*100-100,"")</f>
-        <v>7.5225171672217925</v>
+        <v>8.3240180675480104</v>
       </c>
       <c r="DE8" s="54">
         <f>IFERROR('Tabel 5'!DE8/'Tabel 5'!CS8*100-100,"")</f>
-        <v>-100</v>
+        <v>4.301928384228475</v>
       </c>
       <c r="DF8" s="66" t="s">
         <v>41</v>
@@ -28123,11 +28170,11 @@
       </c>
       <c r="DD9" s="58">
         <f>IFERROR('Tabel 5'!DD9/'Tabel 5'!CR9*100-100,"")</f>
-        <v>-14.394252933448641</v>
+        <v>-15.236639360289701</v>
       </c>
       <c r="DE9" s="58">
         <f>IFERROR('Tabel 5'!DE9/'Tabel 5'!CS9*100-100,"")</f>
-        <v>-100</v>
+        <v>-15.448399885888477</v>
       </c>
       <c r="DF9" s="67" t="s">
         <v>42</v>
@@ -28551,11 +28598,11 @@
       </c>
       <c r="DD10" s="54">
         <f>IFERROR('Tabel 5'!DD10/'Tabel 5'!CR10*100-100,"")</f>
-        <v>-29.833582983895624</v>
+        <v>-34.127142545353109</v>
       </c>
       <c r="DE10" s="54">
         <f>IFERROR('Tabel 5'!DE10/'Tabel 5'!CS10*100-100,"")</f>
-        <v>-100</v>
+        <v>-34.802662236041897</v>
       </c>
       <c r="DF10" s="66" t="s">
         <v>43</v>
@@ -28979,11 +29026,11 @@
       </c>
       <c r="DD11" s="58">
         <f>IFERROR('Tabel 5'!DD11/'Tabel 5'!CR11*100-100,"")</f>
-        <v>-10.492537576888495</v>
+        <v>-15.253588203803417</v>
       </c>
       <c r="DE11" s="58">
         <f>IFERROR('Tabel 5'!DE11/'Tabel 5'!CS11*100-100,"")</f>
-        <v>-100</v>
+        <v>-14.435608062975746</v>
       </c>
       <c r="DF11" s="67" t="s">
         <v>44</v>
@@ -29407,11 +29454,11 @@
       </c>
       <c r="DD12" s="54">
         <f>IFERROR('Tabel 5'!DD12/'Tabel 5'!CR12*100-100,"")</f>
-        <v>1.6451878407630574</v>
+        <v>-0.14389619325714875</v>
       </c>
       <c r="DE12" s="54">
         <f>IFERROR('Tabel 5'!DE12/'Tabel 5'!CS12*100-100,"")</f>
-        <v>-100</v>
+        <v>-6.9967641928681701</v>
       </c>
       <c r="DF12" s="66" t="s">
         <v>45</v>
@@ -29835,11 +29882,11 @@
       </c>
       <c r="DD13" s="58">
         <f>IFERROR('Tabel 5'!DD13/'Tabel 5'!CR13*100-100,"")</f>
-        <v>7.9327099426880494</v>
+        <v>9.0933065205084773</v>
       </c>
       <c r="DE13" s="58">
         <f>IFERROR('Tabel 5'!DE13/'Tabel 5'!CS13*100-100,"")</f>
-        <v>-100</v>
+        <v>0.89653722037081707</v>
       </c>
       <c r="DF13" s="67" t="s">
         <v>46</v>
@@ -30263,11 +30310,11 @@
       </c>
       <c r="DD14" s="54">
         <f>IFERROR('Tabel 5'!DD14/'Tabel 5'!CR14*100-100,"")</f>
-        <v>-31.723799399825182</v>
+        <v>-31.994173261758192</v>
       </c>
       <c r="DE14" s="54">
         <f>IFERROR('Tabel 5'!DE14/'Tabel 5'!CS14*100-100,"")</f>
-        <v>-100</v>
+        <v>-32.842656844319933</v>
       </c>
       <c r="DF14" s="66" t="s">
         <v>47</v>
@@ -30691,11 +30738,11 @@
       </c>
       <c r="DD15" s="62">
         <f>IFERROR('Tabel 5'!DD15/'Tabel 5'!CR15*100-100,"")</f>
-        <v>-15.659859886113878</v>
+        <v>-16.273595016147354</v>
       </c>
       <c r="DE15" s="62">
         <f>IFERROR('Tabel 5'!DE15/'Tabel 5'!CS15*100-100,"")</f>
-        <v>-100</v>
+        <v>-20.658013732269211</v>
       </c>
       <c r="DF15" s="80" t="s">
         <v>31</v>
@@ -30782,7 +30829,7 @@
       <c r="DG18" s="37"/>
       <c r="DH18" s="37"/>
     </row>
-    <row r="19" spans="1:112" s="20" customFormat="1" ht="13.5">
+    <row r="19" spans="1:112" s="20" customFormat="1" ht="13.2">
       <c r="A19" s="22" t="s">
         <v>83</v>
       </c>
@@ -30814,21 +30861,20 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DC5" sqref="DC5:DD5"/>
+      <selection pane="topRight" activeCell="DD6" sqref="DD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="61" width="9.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="9.08984375" collapsed="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="61" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="9.109375" collapsed="1"/>
     <col min="76" max="76" width="8" customWidth="1"/>
-    <col min="77" max="77" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="80" max="91" width="9.08984375" customWidth="1"/>
-    <col min="92" max="92" width="9.81640625" customWidth="1"/>
-    <col min="93" max="108" width="9.08984375" customWidth="1"/>
-    <col min="109" max="109" width="9.08984375" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="28.453125" customWidth="1"/>
+    <col min="77" max="77" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="91" width="9.109375" customWidth="1"/>
+    <col min="92" max="92" width="9.77734375" customWidth="1"/>
+    <col min="93" max="109" width="9.109375" customWidth="1"/>
+    <col min="110" max="110" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:110" s="16" customFormat="1" ht="15" customHeight="1">
@@ -31447,7 +31493,7 @@
         <v>9</v>
       </c>
       <c r="DD5" s="50" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="DE5" s="51" t="s">
         <v>86</v>
@@ -31883,11 +31929,11 @@
       </c>
       <c r="DD6" s="54">
         <f>IFERROR('Tabel 5'!DD6/'Tabel 5'!DC6*100-100,"")</f>
-        <v>4.1473866618010504</v>
+        <v>3.0667905841415148</v>
       </c>
       <c r="DE6" s="54">
         <f>IFERROR('Tabel 5'!DE6/'Tabel 5'!DD6*100-100,"")</f>
-        <v>-100</v>
+        <v>10.65757045752224</v>
       </c>
       <c r="DF6" s="66" t="s">
         <v>39</v>
@@ -32322,11 +32368,11 @@
       </c>
       <c r="DD7" s="58">
         <f>IFERROR('Tabel 5'!DD7/'Tabel 5'!DC7*100-100,"")</f>
-        <v>-4.7175591096372216</v>
+        <v>-4.8837869189253098</v>
       </c>
       <c r="DE7" s="58">
         <f>IFERROR('Tabel 5'!DE7/'Tabel 5'!DD7*100-100,"")</f>
-        <v>-100</v>
+        <v>0.96067750051378198</v>
       </c>
       <c r="DF7" s="67" t="s">
         <v>40</v>
@@ -32761,11 +32807,11 @@
       </c>
       <c r="DD8" s="54">
         <f>IFERROR('Tabel 5'!DD8/'Tabel 5'!DC8*100-100,"")</f>
-        <v>2.9712208278823482</v>
+        <v>3.7387951776614017</v>
       </c>
       <c r="DE8" s="54">
         <f>IFERROR('Tabel 5'!DE8/'Tabel 5'!DD8*100-100,"")</f>
-        <v>-100</v>
+        <v>2.9425638946319026</v>
       </c>
       <c r="DF8" s="66" t="s">
         <v>41</v>
@@ -33200,11 +33246,11 @@
       </c>
       <c r="DD9" s="58">
         <f>IFERROR('Tabel 5'!DD9/'Tabel 5'!DC9*100-100,"")</f>
-        <v>2.8165081837033625</v>
+        <v>1.8047626652416966</v>
       </c>
       <c r="DE9" s="58">
         <f>IFERROR('Tabel 5'!DE9/'Tabel 5'!DD9*100-100,"")</f>
-        <v>-100</v>
+        <v>3.2677190369602158</v>
       </c>
       <c r="DF9" s="67" t="s">
         <v>42</v>
@@ -33639,11 +33685,11 @@
       </c>
       <c r="DD10" s="54">
         <f>IFERROR('Tabel 5'!DD10/'Tabel 5'!DC10*100-100,"")</f>
-        <v>-1.8251838658147221</v>
+        <v>-7.8326079075826698</v>
       </c>
       <c r="DE10" s="54">
         <f>IFERROR('Tabel 5'!DE10/'Tabel 5'!DD10*100-100,"")</f>
-        <v>-100</v>
+        <v>4.6214615440078859</v>
       </c>
       <c r="DF10" s="66" t="s">
         <v>43</v>
@@ -34078,11 +34124,11 @@
       </c>
       <c r="DD11" s="58">
         <f>IFERROR('Tabel 5'!DD11/'Tabel 5'!DC11*100-100,"")</f>
-        <v>4.5979737302542105</v>
+        <v>-0.96576626327141923</v>
       </c>
       <c r="DE11" s="58">
         <f>IFERROR('Tabel 5'!DE11/'Tabel 5'!DD11*100-100,"")</f>
-        <v>-100</v>
+        <v>6.7099407716547859</v>
       </c>
       <c r="DF11" s="67" t="s">
         <v>44</v>
@@ -34517,11 +34563,11 @@
       </c>
       <c r="DD12" s="54">
         <f>IFERROR('Tabel 5'!DD12/'Tabel 5'!DC12*100-100,"")</f>
-        <v>0.98785659339131371</v>
+        <v>-0.7896575782013997</v>
       </c>
       <c r="DE12" s="54">
         <f>IFERROR('Tabel 5'!DE12/'Tabel 5'!DD12*100-100,"")</f>
-        <v>-100</v>
+        <v>2.1420878574956532</v>
       </c>
       <c r="DF12" s="66" t="s">
         <v>45</v>
@@ -34956,11 +35002,11 @@
       </c>
       <c r="DD13" s="58">
         <f>IFERROR('Tabel 5'!DD13/'Tabel 5'!DC13*100-100,"")</f>
-        <v>1.4384687062451746</v>
+        <v>2.5292329398341167</v>
       </c>
       <c r="DE13" s="58">
         <f>IFERROR('Tabel 5'!DE13/'Tabel 5'!DD13*100-100,"")</f>
-        <v>-100</v>
+        <v>4.6216259171383882</v>
       </c>
       <c r="DF13" s="67" t="s">
         <v>46</v>
@@ -35395,11 +35441,11 @@
       </c>
       <c r="DD14" s="54">
         <f>IFERROR('Tabel 5'!DD14/'Tabel 5'!DC14*100-100,"")</f>
-        <v>-0.38008979874028626</v>
+        <v>-0.77458480006970376</v>
       </c>
       <c r="DE14" s="54">
         <f>IFERROR('Tabel 5'!DE14/'Tabel 5'!DD14*100-100,"")</f>
-        <v>-100</v>
+        <v>0.75931629331600448</v>
       </c>
       <c r="DF14" s="66" t="s">
         <v>47</v>
@@ -35834,11 +35880,11 @@
       </c>
       <c r="DD15" s="62">
         <f>IFERROR('Tabel 5'!DD15/'Tabel 5'!DC15*100-100,"")</f>
-        <v>-0.43964726430503731</v>
+        <v>-1.16413842533359</v>
       </c>
       <c r="DE15" s="62">
         <f>IFERROR('Tabel 5'!DE15/'Tabel 5'!DD15*100-100,"")</f>
-        <v>-100</v>
+        <v>2.8651901604154233</v>
       </c>
       <c r="DF15" s="80" t="s">
         <v>31</v>
@@ -35923,7 +35969,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:110" s="20" customFormat="1" ht="13.5">
+    <row r="19" spans="1:110" s="20" customFormat="1" ht="13.2">
       <c r="A19" s="22" t="s">
         <v>83</v>
       </c>
@@ -35958,22 +36004,21 @@
       <pane xSplit="1" ySplit="5" topLeftCell="Z6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ6" sqref="AJ6"/>
+      <selection pane="bottomRight" activeCell="AK6" sqref="AK6:AK15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="16" width="9.08984375" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="9.453125" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="21" width="9.08984375" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.08984375"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="16" width="9.109375" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="9.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="21" width="9.109375" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.109375"/>
     <col min="26" max="26" width="8" style="48" customWidth="1"/>
-    <col min="27" max="27" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.81640625" customWidth="1"/>
-    <col min="29" max="36" width="7.54296875" customWidth="1"/>
-    <col min="37" max="37" width="7.54296875" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="27.6328125" customWidth="1"/>
+    <col min="27" max="27" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.77734375" customWidth="1"/>
+    <col min="29" max="37" width="7.5546875" customWidth="1"/>
+    <col min="38" max="38" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:38" s="16" customFormat="1" ht="15" customHeight="1">
@@ -36327,7 +36372,9 @@
         <f>AVERAGE('Tabel 6'!CZ6:DB6)</f>
         <v>-45.155620862648256</v>
       </c>
-      <c r="AK6" s="117"/>
+      <c r="AK6" s="117">
+        <v>-46.709124190613238</v>
+      </c>
       <c r="AL6" s="66" t="s">
         <v>39</v>
       </c>
@@ -36448,7 +36495,9 @@
         <f>AVERAGE('Tabel 6'!CZ7:DB7)</f>
         <v>-16.751899893435223</v>
       </c>
-      <c r="AK7" s="118"/>
+      <c r="AK7" s="118">
+        <v>-29.738874313077066</v>
+      </c>
       <c r="AL7" s="67" t="s">
         <v>40</v>
       </c>
@@ -36569,7 +36618,9 @@
         <f>AVERAGE('Tabel 6'!CZ8:DB8)</f>
         <v>4.7802587082615604</v>
       </c>
-      <c r="AK8" s="117"/>
+      <c r="AK8" s="117">
+        <v>5.8937281567673345</v>
+      </c>
       <c r="AL8" s="66" t="s">
         <v>41</v>
       </c>
@@ -36690,7 +36741,9 @@
         <f>AVERAGE('Tabel 6'!CZ9:DB9)</f>
         <v>-18.930803518680332</v>
       </c>
-      <c r="AK9" s="118"/>
+      <c r="AK9" s="118">
+        <v>-15.31274794462861</v>
+      </c>
       <c r="AL9" s="67" t="s">
         <v>42</v>
       </c>
@@ -36811,7 +36864,9 @@
         <f>AVERAGE('Tabel 6'!CZ10:DB10)</f>
         <v>-11.385451927993321</v>
       </c>
-      <c r="AK10" s="117"/>
+      <c r="AK10" s="117">
+        <v>-31.516014726161217</v>
+      </c>
       <c r="AL10" s="66" t="s">
         <v>43</v>
       </c>
@@ -36932,7 +36987,9 @@
         <f>AVERAGE('Tabel 6'!CZ11:DB11)</f>
         <v>-37.182211334960236</v>
       </c>
-      <c r="AK11" s="118"/>
+      <c r="AK11" s="118">
+        <v>-14.453126212028161</v>
+      </c>
       <c r="AL11" s="67" t="s">
         <v>44</v>
       </c>
@@ -37053,7 +37110,9 @@
         <f>AVERAGE('Tabel 6'!CZ12:DB12)</f>
         <v>3.1305947185759067</v>
       </c>
-      <c r="AK12" s="117"/>
+      <c r="AK12" s="117">
+        <v>-1.210486251152924</v>
+      </c>
       <c r="AL12" s="66" t="s">
         <v>45</v>
       </c>
@@ -37174,7 +37233,9 @@
         <f>AVERAGE('Tabel 6'!CZ13:DB13)</f>
         <v>9.8673906107254172</v>
       </c>
-      <c r="AK13" s="118"/>
+      <c r="AK13" s="118">
+        <v>5.3958420807904472</v>
+      </c>
       <c r="AL13" s="67" t="s">
         <v>46</v>
       </c>
@@ -37295,7 +37356,9 @@
         <f>AVERAGE('Tabel 6'!CZ14:DB14)</f>
         <v>-31.814601509990087</v>
       </c>
-      <c r="AK14" s="117"/>
+      <c r="AK14" s="117">
+        <v>-31.98683744000952</v>
+      </c>
       <c r="AL14" s="66" t="s">
         <v>47</v>
       </c>
@@ -37416,7 +37479,9 @@
         <f>AVERAGE('Tabel 6'!CZ15:DB15)</f>
         <v>-10.06733208233031</v>
       </c>
-      <c r="AK15" s="119"/>
+      <c r="AK15" s="119">
+        <v>-17.292126116453691</v>
+      </c>
       <c r="AL15" s="68" t="s">
         <v>31</v>
       </c>
@@ -37551,19 +37616,19 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="CR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CY18" sqref="CY18"/>
+      <selection pane="topRight" activeCell="DF18" sqref="DF18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="61" width="9.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="8.90625" collapsed="1"/>
-    <col min="80" max="82" width="9.08984375" customWidth="1"/>
-    <col min="83" max="83" width="9.36328125" customWidth="1"/>
-    <col min="84" max="107" width="9.08984375" customWidth="1"/>
-    <col min="108" max="109" width="9.08984375" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="36.453125" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="61" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="8.88671875" collapsed="1"/>
+    <col min="80" max="82" width="9.109375" customWidth="1"/>
+    <col min="83" max="83" width="9.33203125" customWidth="1"/>
+    <col min="84" max="108" width="9.109375" customWidth="1"/>
+    <col min="109" max="109" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="110" max="110" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:110" s="16" customFormat="1" ht="14.4" customHeight="1">
@@ -38882,7 +38947,9 @@
       <c r="DC8" s="92">
         <v>139.78317332402952</v>
       </c>
-      <c r="DD8" s="92"/>
+      <c r="DD8" s="92">
+        <v>150.41121413382052</v>
+      </c>
       <c r="DE8" s="92"/>
       <c r="DF8" s="94" t="s">
         <v>53</v>
@@ -39287,7 +39354,9 @@
       <c r="DC9" s="92">
         <v>163.91653279846034</v>
       </c>
-      <c r="DD9" s="92"/>
+      <c r="DD9" s="92">
+        <v>161.66314188571283</v>
+      </c>
       <c r="DE9" s="92"/>
       <c r="DF9" s="94" t="s">
         <v>54</v>
@@ -39920,7 +39989,9 @@
       <c r="DC12" s="92">
         <v>151.55844155844159</v>
       </c>
-      <c r="DD12" s="92"/>
+      <c r="DD12" s="92">
+        <v>153.43709468223088</v>
+      </c>
       <c r="DE12" s="92"/>
       <c r="DF12" s="94" t="s">
         <v>53</v>
@@ -40325,7 +40396,9 @@
       <c r="DC13" s="92">
         <v>160.51948051948051</v>
       </c>
-      <c r="DD13" s="92"/>
+      <c r="DD13" s="92">
+        <v>165.06493506493507</v>
+      </c>
       <c r="DE13" s="92"/>
       <c r="DF13" s="94" t="s">
         <v>54</v>

</xml_diff>